<commit_message>
Translating project to english and adding relevant information to README file.
</commit_message>
<xml_diff>
--- a/data/aux/exchange_rates.xlsx
+++ b/data/aux/exchange_rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloseduardogomeztorres/Desktop/BIA/TFG/data/aux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38449FD6-8E61-7C4B-A749-69A30B0FC056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75194C64-6ABD-6C42-8B8D-CBC781B5275A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="640" windowWidth="26440" windowHeight="14940" xr2:uid="{C1D96804-815C-2046-AB0A-6058A02D3F45}"/>
+    <workbookView xWindow="2360" yWindow="640" windowWidth="26440" windowHeight="14940" xr2:uid="{C1D96804-815C-2046-AB0A-6058A02D3F45}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Año</t>
+    <t>rate</t>
   </si>
   <si>
-    <t>rate</t>
+    <t>YEAR</t>
   </si>
 </sst>
 </file>
@@ -416,17 +416,17 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>